<commit_message>
Update playlist and detail
</commit_message>
<xml_diff>
--- a/data/songs.xlsx
+++ b/data/songs.xlsx
@@ -569,6 +569,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -591,6 +592,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -734,16 +736,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="106.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="117.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="117.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,10 +886,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.35"/>
@@ -1039,7 +1041,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
@@ -1059,7 +1061,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -1079,7 +1081,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -1099,7 +1101,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
@@ -1119,7 +1121,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -1139,7 +1141,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2</v>
@@ -1159,7 +1161,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>3</v>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
@@ -1199,7 +1201,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
@@ -1219,7 +1221,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3</v>
@@ -1239,7 +1241,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -1259,7 +1261,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
@@ -1279,7 +1281,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
@@ -1299,7 +1301,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
@@ -1319,7 +1321,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>4</v>
@@ -1339,7 +1341,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>4</v>
@@ -1359,7 +1361,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>4</v>
@@ -1379,7 +1381,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -1399,7 +1401,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>4</v>
@@ -1419,7 +1421,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>4</v>
@@ -1439,7 +1441,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>4</v>
@@ -1459,7 +1461,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>5</v>
@@ -1479,7 +1481,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>5</v>
@@ -1499,7 +1501,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>5</v>
@@ -1519,7 +1521,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>5</v>
@@ -1539,7 +1541,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5</v>
@@ -1559,7 +1561,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -1579,7 +1581,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -1599,7 +1601,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>6</v>
@@ -1619,7 +1621,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>6</v>
@@ -1639,7 +1641,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>6</v>
@@ -1659,7 +1661,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>6</v>
@@ -1679,7 +1681,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
[#4] Add playlist and song detail (#13)
* Add playlist screen
* Add initial playing song detail
</commit_message>
<xml_diff>
--- a/data/songs.xlsx
+++ b/data/songs.xlsx
@@ -569,6 +569,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -591,6 +592,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -734,16 +736,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="106.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="117.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="117.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,10 +886,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.35"/>
@@ -1039,7 +1041,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
@@ -1059,7 +1061,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -1079,7 +1081,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
@@ -1099,7 +1101,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
@@ -1119,7 +1121,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2</v>
@@ -1139,7 +1141,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2</v>
@@ -1159,7 +1161,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>3</v>
@@ -1179,7 +1181,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
@@ -1199,7 +1201,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
@@ -1219,7 +1221,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3</v>
@@ -1239,7 +1241,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -1259,7 +1261,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
@@ -1279,7 +1281,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
@@ -1299,7 +1301,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
@@ -1319,7 +1321,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>4</v>
@@ -1339,7 +1341,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>4</v>
@@ -1359,7 +1361,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>4</v>
@@ -1379,7 +1381,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
@@ -1399,7 +1401,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>4</v>
@@ -1419,7 +1421,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>4</v>
@@ -1439,7 +1441,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>4</v>
@@ -1459,7 +1461,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>5</v>
@@ -1479,7 +1481,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>5</v>
@@ -1499,7 +1501,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>5</v>
@@ -1519,7 +1521,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>5</v>
@@ -1539,7 +1541,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5</v>
@@ -1559,7 +1561,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>5</v>
@@ -1579,7 +1581,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>6</v>
@@ -1599,7 +1601,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>6</v>
@@ -1619,7 +1621,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>6</v>
@@ -1639,7 +1641,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>6</v>
@@ -1659,7 +1661,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>6</v>
@@ -1679,7 +1681,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Fix bugs and update packages
</commit_message>
<xml_diff>
--- a/data/songs.xlsx
+++ b/data/songs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="182">
   <si>
     <t xml:space="preserve">no</t>
   </si>
@@ -555,6 +555,18 @@
   </si>
   <si>
     <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/c5/Dev-masali-cizim.png/300px-Dev-masali-cizim.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neşeli Bir Gün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ne%C5%9Feli_Bir_G%C3%BCn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/5/53/Ne%C5%9Feli_Bir_G%C3%BCn.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/subadap-cocuk-logo_w125.png?d57f9</t>
   </si>
 </sst>
 </file>
@@ -643,16 +655,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -729,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -742,26 +758,26 @@
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="25.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="106.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="117.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="106.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="117.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -769,16 +785,16 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2014</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -786,16 +802,16 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -803,16 +819,16 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -820,16 +836,16 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2017</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -837,16 +853,16 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -854,16 +870,16 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -879,824 +895,841 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="79.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="130.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="135.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="79.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="130.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="135.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="2" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#82] Update UI components (#83)
Closes #82
</commit_message>
<xml_diff>
--- a/data/songs.xlsx
+++ b/data/songs.xlsx
@@ -101,472 +101,472 @@
     <t xml:space="preserve">Düş</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/D%C3%BC%C5%9F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/1/1e/D%C3%BC%C5%9F.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/e/e9/D%C3%BC%C5%9F-r.png/300px-D%C3%BC%C5%9F-r.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/D%C3%BC%C5%9F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/1/1e/D%C3%BC%C5%9F.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/e/e9/D%C3%BC%C5%9F-r.png/300px-D%C3%BC%C5%9F-r.png</t>
   </si>
   <si>
     <t xml:space="preserve">Bomba Yapan Bay Bilgin</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Bomba_Yapan_Bay_Bilgin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/d/dc/Bomba_yapan_bay_bilgin.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/9/93/Bomba_yapan_R.png/300px-Bomba_yapan_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Bomba_Yapan_Bay_Bilgin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/d/dc/Bomba_yapan_bay_bilgin.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/9/93/Bomba_yapan_R.png/300px-Bomba_yapan_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Her Yer Park Olsa</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Her_Yer_Park_Olsa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/4/40/Her_Yer_Park_Olsa.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/c7/Her_yer_park_olsa.png/300px-Her_yer_park_olsa.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Her_Yer_Park_Olsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/4/40/Her_Yer_Park_Olsa.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/c7/Her_yer_park_olsa.png/300px-Her_yer_park_olsa.png</t>
   </si>
   <si>
     <t xml:space="preserve">Kalem Kağıt</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Kalem_Ka%C4%9F%C4%B1t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/5/56/Kalem_K%C3%A2%C4%9F%C4%B1t.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/7/74/Kalem_ka%C4%9F%C4%B1t_R.png/300px-Kalem_ka%C4%9F%C4%B1t_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Kalem_Ka%C4%9F%C4%B1t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/5/56/Kalem_K%C3%A2%C4%9F%C4%B1t.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/7/74/Kalem_ka%C4%9F%C4%B1t_R.png/300px-Kalem_ka%C4%9F%C4%B1t_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Uzaylı Arkadaşım</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Uzayl%C4%B1_Arkada%C5%9F%C4%B1m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/b/b3/Uzayl%C4%B1_Arkada%C5%9F%C4%B1m.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/8/8f/Uzayl%C4%B1_arkada%C5%9F%C4%B1m_R.png/300px-Uzayl%C4%B1_arkada%C5%9F%C4%B1m_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Uzayl%C4%B1_Arkada%C5%9F%C4%B1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/b/b3/Uzayl%C4%B1_Arkada%C5%9F%C4%B1m.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/8/8f/Uzayl%C4%B1_arkada%C5%9F%C4%B1m_R.png/300px-Uzayl%C4%B1_arkada%C5%9F%C4%B1m_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Şubadap Şubi</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/%C5%9Eubadap_%C5%9Eubi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/7/7e/%C5%9Eubadap.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/4/4a/%C5%9Eubadap_R.png/300px-%C5%9Eubadap_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/%C5%9Eubadap_%C5%9Eubi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/7/7e/%C5%9Eubadap.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/4/4a/%C5%9Eubadap_R.png/300px-%C5%9Eubadap_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Ben Doğmadan Önce</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ben_Do%C4%9Fmadan_%C3%96nce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/3/3a/Ben_dogmadan_once.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/1/11/Ben_do%C4%9Fmadan.png/300px-Ben_do%C4%9Fmadan.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ben_Do%C4%9Fmadan_%C3%96nce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/3/3a/Ben_dogmadan_once.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/1/11/Ben_do%C4%9Fmadan.png/300px-Ben_do%C4%9Fmadan.png</t>
   </si>
   <si>
     <t xml:space="preserve">Yaşam Ağacı</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ya%C5%9Fam_A%C4%9Fac%C4%B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/f/f9/Yasam_A%C4%9Fac%C4%B1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/9/9b/Ya%C5%9Fam_a%C4%9Fac%C4%B1_R.png/300px-Ya%C5%9Fam_a%C4%9Fac%C4%B1_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ya%C5%9Fam_A%C4%9Fac%C4%B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/f/f9/Yasam_A%C4%9Fac%C4%B1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/9/9b/Ya%C5%9Fam_a%C4%9Fac%C4%B1_R.png/300px-Ya%C5%9Fam_a%C4%9Fac%C4%B1_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Dino’nun Şarkısı</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Dino%27nun_%C5%9Eark%C4%B1s%C4%B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/4/41/Dinonun_%C5%9Eark%C4%B1s%C4%B1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/d/d3/Dinonun_%C5%9Fark%C4%B1s%C4%B1_R.png/300px-Dinonun_%C5%9Fark%C4%B1s%C4%B1_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Dino%27nun_%C5%9Eark%C4%B1s%C4%B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/4/41/Dinonun_%C5%9Eark%C4%B1s%C4%B1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/d/d3/Dinonun_%C5%9Fark%C4%B1s%C4%B1_R.png/300px-Dinonun_%C5%9Fark%C4%B1s%C4%B1_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Ornitorenk</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ornitorenk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/c/cb/Ornitorenk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/0/05/Ornitorenk_R.png/300px-Ornitorenk_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ornitorenk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/c/cb/Ornitorenk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/0/05/Ornitorenk_R.png/300px-Ornitorenk_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Zaman Makinesi</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Zaman_Makinesi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/5/5c/Zaman_Makinesi.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/2/2a/Zaman_makinesi_R.png/300px-Zaman_makinesi_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Zaman_Makinesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/5/5c/Zaman_Makinesi.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/2/2a/Zaman_makinesi_R.png/300px-Zaman_makinesi_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Değişelim</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/De%C4%9Fi%C5%9Felim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/9/94/Degiselim.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/1/1b/De%C4%9Fi%C5%9Felim.png/300px-De%C4%9Fi%C5%9Felim.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/De%C4%9Fi%C5%9Felim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/9/94/Degiselim.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/1/1b/De%C4%9Fi%C5%9Felim.png/300px-De%C4%9Fi%C5%9Felim.png</t>
   </si>
   <si>
     <t xml:space="preserve">Çekirdeksiz Domates</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/%C3%87ekirdeksiz_Domates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/6/62/%C3%87ekirdeksiz_Domates.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/7/76/%C3%87ekirdeksiz_R.png/300px-%C3%87ekirdeksiz_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/%C3%87ekirdeksiz_Domates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/6/62/%C3%87ekirdeksiz_Domates.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/7/76/%C3%87ekirdeksiz_R.png/300px-%C3%87ekirdeksiz_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Su</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Su</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/2/22/Su.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/3/30/Su_R.png/300px-Su_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Su</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/2/22/Su.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/3/30/Su_R.png/300px-Su_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Irmaklar Özgür Akacak</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Irmaklar_%C3%96zg%C3%BCr_Akacak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/5/57/Irmaklar_%C3%96zg%C3%BCr_Akacak.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/f/f1/Irmaklar_%C3%B6zg%C3%BCr_R.png/300px-Irmaklar_%C3%B6zg%C3%BCr_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Irmaklar_%C3%96zg%C3%BCr_Akacak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/5/57/Irmaklar_%C3%96zg%C3%BCr_Akacak.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/f/f1/Irmaklar_%C3%B6zg%C3%BCr_R.png/300px-Irmaklar_%C3%B6zg%C3%BCr_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Zeytin Ağacı</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Zeytin_A%C4%9Fac%C4%B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/4/47/Zeytin_A%C4%9Fac%C4%B1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/c7/Zeytin_a%C4%9Fac%C4%B1_R.png/300px-Zeytin_a%C4%9Fac%C4%B1_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Zeytin_A%C4%9Fac%C4%B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/4/47/Zeytin_A%C4%9Fac%C4%B1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/c7/Zeytin_a%C4%9Fac%C4%B1_R.png/300px-Zeytin_a%C4%9Fac%C4%B1_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Sivrisinek</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Sivrisinek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/2/22/Sivrisinek.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/2/2c/Sivrisinek_R.png/300px-Sivrisinek_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Sivrisinek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/2/22/Sivrisinek.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/2/2c/Sivrisinek_R.png/300px-Sivrisinek_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Kurbağa Korosu</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Kurba%C4%9Fa_Korosu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/a/ac/Kurba%C4%9Fa_Korosu.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/6/69/Kurba%C4%9Fa_korosu_R.png/300px-Kurba%C4%9Fa_korosu_R.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Kurba%C4%9Fa_Korosu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/a/ac/Kurba%C4%9Fa_Korosu.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/6/69/Kurba%C4%9Fa_korosu_R.png/300px-Kurba%C4%9Fa_korosu_R.png</t>
   </si>
   <si>
     <t xml:space="preserve">Dinleyin Paragözler</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Dinleyin_Parag%C3%B6zler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/b/b3/Dinleyin_Parag%C3%B6zler.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/6/67/Dinleyin_parag%C3%B6zler_R.png/300px-Dinleyin_parag%C3%B6zler_R.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/G%C3%B6ky%C3%BCz%C3%BC_Kimin%3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/b/b8/G%C3%B6ky%C3%BCz%C3%BC_Kimin.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/f/f0/G%C3%B6ky%C3%BCz%C3%BC_Kimin_r.png/300px-G%C3%B6ky%C3%BCz%C3%BC_Kimin_r.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Dinleyin_Parag%C3%B6zler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/b/b3/Dinleyin_Parag%C3%B6zler.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/6/67/Dinleyin_parag%C3%B6zler_R.png/300px-Dinleyin_parag%C3%B6zler_R.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/G%C3%B6ky%C3%BCz%C3%BC_Kimin%3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/b/b8/G%C3%B6ky%C3%BCz%C3%BC_Kimin.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/f/f0/G%C3%B6ky%C3%BCz%C3%BC_Kimin_r.png/300px-G%C3%B6ky%C3%BCz%C3%BC_Kimin_r.png</t>
   </si>
   <si>
     <t xml:space="preserve">Özgürlük</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/%C3%96zg%C3%BCrl%C3%BCk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/6/64/Ozgurluk_sarki.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/f/f4/%C3%96zg%C3%BCrl%C3%BCk_R.jpg/300px-%C3%96zg%C3%BCrl%C3%BCk_R.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/%C3%96zg%C3%BCrl%C3%BCk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/6/64/Ozgurluk_sarki.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/f/f4/%C3%96zg%C3%BCrl%C3%BCk_R.jpg/300px-%C3%96zg%C3%BCrl%C3%BCk_R.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Elmer</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Elmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/9/91/Elmer.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/0/0c/Elmerburr.jpg/300px-Elmerburr.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Elmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/9/91/Elmer.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/0/0c/Elmerburr.jpg/300px-Elmerburr.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Karınca</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Kar%C4%B1nca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/f/f4/Kar%C4%B1nca.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/e/e6/Kar%C4%B1ncalar_R.jpg/300px-Kar%C4%B1ncalar_R.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Kar%C4%B1nca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/f/f4/Kar%C4%B1nca.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/e/e6/Kar%C4%B1ncalar_R.jpg/300px-Kar%C4%B1ncalar_R.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Zorba</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Zorba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/0/06/Zorba.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/3/31/Zorba_R.jpg/300px-Zorba_R.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Zorba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/0/06/Zorba.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/3/31/Zorba_R.jpg/300px-Zorba_R.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Uçurtma</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/U%C3%A7urtma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/4/40/Ucurtma_sarki.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/8/81/U%C3%A7urtma_R.jpg/300px-U%C3%A7urtma_R.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/U%C3%A7urtma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/4/40/Ucurtma_sarki.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/8/81/U%C3%A7urtma_R.jpg/300px-U%C3%A7urtma_R.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Ne Olsam?</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ne_Olsam%3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/b/b4/Ne_Olsam_%C5%9Fark%C4%B1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/3/3b/Ne_olsam_R.jpg/300px-Ne_olsam_R.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Dersler_Uzun_Teneff%C3%BCsler_K%C4%B1sa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/3/3f/Dersler-uzun-Teneff%C3%BCsler-K%C4%B1sa.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/d/da/Dutk_R.jpg/300px-Dutk_R.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ne_Olsam%3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/b/b4/Ne_Olsam_%C5%9Fark%C4%B1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/3/3b/Ne_olsam_R.jpg/300px-Ne_olsam_R.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Dersler_Uzun_Teneff%C3%BCsler_K%C4%B1sa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/3/3f/Dersler-uzun-Teneff%C3%BCsler-K%C4%B1sa.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/d/da/Dutk_R.jpg/300px-Dutk_R.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Fasa Fiso</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Fasa_Fiso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/1/19/Fasa-Fiso-%C5%9Eubadap-%C3%87ocuk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/9/9a/Faso-fiso.jpg/300px-Faso-fiso.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Fasa_Fiso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/1/19/Fasa-Fiso-%C5%9Eubadap-%C3%87ocuk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/9/9a/Faso-fiso.jpg/300px-Faso-fiso.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Makine Çocuk</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Makine_%C3%87ocuk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/0/04/Makine-%C3%87ocuk-%C5%9Eubadap-%C3%87ocuk_1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/4/44/Makine-%C3%A7ocuk2.jpg/300px-Makine-%C3%A7ocuk2.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Makine_%C3%87ocuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/0/04/Makine-%C3%87ocuk-%C5%9Eubadap-%C3%87ocuk_1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/4/44/Makine-%C3%A7ocuk2.jpg/300px-Makine-%C3%A7ocuk2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Serçe</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ser%C3%A7e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/9/93/Ser%C3%A7e_-_%C5%9Eubadap_%C3%87ocuk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/9/9f/Ser%C3%A7e3.jpg/300px-Ser%C3%A7e3.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ser%C3%A7e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/9/93/Ser%C3%A7e_-_%C5%9Eubadap_%C3%87ocuk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/9/9f/Ser%C3%A7e3.jpg/300px-Ser%C3%A7e3.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Çocuk Hakları</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/%C3%87ocuk_Haklar%C4%B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/e/ef/%C3%87ocuk-Haklar%C4%B1-%C5%9Eubadap-%C3%87ocuk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/b/b8/%C3%87ocuk_haklar%C4%B1_resim.png/300px-%C3%87ocuk_haklar%C4%B1_resim.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Hayal_Et</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/2/2e/Hayal-Et-%C5%9Eubadap-%C3%87ocuk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/ce/Hayal-et2.jpg/300px-Hayal-et2.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/%C3%87ocuk_Haklar%C4%B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/e/ef/%C3%87ocuk-Haklar%C4%B1-%C5%9Eubadap-%C3%87ocuk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/b/b8/%C3%87ocuk_haklar%C4%B1_resim.png/300px-%C3%87ocuk_haklar%C4%B1_resim.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Hayal_Et</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/2/2e/Hayal-Et-%C5%9Eubadap-%C3%87ocuk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/ce/Hayal-et2.jpg/300px-Hayal-et2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Gökyüzünü İten Kuş</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/G%C3%B6ky%C3%BCz%C3%BCn%C3%BC_%C4%B0ten_Ku%C5%9F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/7/7d/G%C3%B6ky%C3%BCz%C3%BCn%C3%BC-%C4%B0ten-Ku%C5%9F-%C5%9Eubadap-%C3%87ocuk.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/1/1b/Ku%C5%9F.jpg/300px-Ku%C5%9F.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/G%C3%B6ky%C3%BCz%C3%BCn%C3%BC_%C4%B0ten_Ku%C5%9F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/7/7d/G%C3%B6ky%C3%BCz%C3%BCn%C3%BC-%C4%B0ten-Ku%C5%9F-%C5%9Eubadap-%C3%87ocuk.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/1/1b/Ku%C5%9F.jpg/300px-Ku%C5%9F.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Emek Demek Ne Demek?</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Emek_Demek_Ne_Demek%3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/7/7a/Emek_Demek_Ne_Demek%3F.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/ca/Emek-cizim.jpg/300px-Emek-cizim.jpg</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Emek_Demek_Ne_Demek%3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/7/7a/Emek_Demek_Ne_Demek%3F.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/ca/Emek-cizim.jpg/300px-Emek-cizim.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Bisiklet</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Bisiklet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/9/9e/Bisiklet.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/7/71/Bisiklet-cizim.png/300px-Bisiklet-cizim.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Bisiklet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/9/9e/Bisiklet.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/7/71/Bisiklet-cizim.png/300px-Bisiklet-cizim.png</t>
   </si>
   <si>
     <t xml:space="preserve">Bir Arkadaşım Var</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Bir_Arkada%C5%9F%C4%B1m_Var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/7/71/Bir_Arkada%C5%9F%C4%B1m_Var.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/3/32/Bir-arkadasim-var-cizim2.png/300px-Bir-arkadasim-var-cizim2.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Bir_Arkada%C5%9F%C4%B1m_Var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/7/71/Bir_Arkada%C5%9F%C4%B1m_Var.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/3/32/Bir-arkadasim-var-cizim2.png/300px-Bir-arkadasim-var-cizim2.png</t>
   </si>
   <si>
     <t xml:space="preserve">Ne Fark Eder Ki?</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ne_Fark_Eder_Ki%3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/2/20/Ne_Fark_Eder_Ki%3F.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/c4/Bir-arkadasim-var-cizim.png/300px-Bir-arkadasim-var-cizim.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ne_Fark_Eder_Ki%3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/2/20/Ne_Fark_Eder_Ki%3F.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/c4/Bir-arkadasim-var-cizim.png/300px-Bir-arkadasim-var-cizim.png</t>
   </si>
   <si>
     <t xml:space="preserve">Bana Bir Masal Oku</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Bana_Bir_Masal_Oku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/a/a0/Bana_Bir_Masal_Oku.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/4/49/Bana-bir-masal-oku-cizim.png/300px-Bana-bir-masal-oku-cizim.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Bana_Bir_Masal_Oku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/a/a0/Bana_Bir_Masal_Oku.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/4/49/Bana-bir-masal-oku-cizim.png/300px-Bana-bir-masal-oku-cizim.png</t>
   </si>
   <si>
     <t xml:space="preserve">Dev Masalı</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Dev_Masal%C4%B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/9/92/Dev_Masal%C4%B1.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/thumb/c/c5/Dev-masali-cizim.png/300px-Dev-masali-cizim.png</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Dev_Masal%C4%B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/9/92/Dev_Masal%C4%B1.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/thumb/c/c5/Dev-masali-cizim.png/300px-Dev-masali-cizim.png</t>
   </si>
   <si>
     <t xml:space="preserve">Neşeli Bir Gün</t>
   </si>
   <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/index.php/Ne%C5%9Feli_Bir_G%C3%BCn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/5/53/Ne%C5%9Feli_Bir_G%C3%BCn.mp3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ansiklopedi.subadapcocuk.org/images/subadap-cocuk-logo_w125.png?d57f9</t>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/index.php/Ne%C5%9Feli_Bir_G%C3%BCn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/5/53/Ne%C5%9Feli_Bir_G%C3%BCn.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ansiklopedi.subadapcocuk.org/images/subadap-cocuk-logo_w125.png?d57f9</t>
   </si>
 </sst>
 </file>
@@ -901,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>